<commit_message>
뭔가 된다git add .
</commit_message>
<xml_diff>
--- a/lab5/translation.xlsx
+++ b/lab5/translation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="288">
   <si>
     <t>0. pc &lt;- 35</t>
   </si>
@@ -176,9 +176,6 @@
     <t>174. $2 &lt;- $2 + 1</t>
   </si>
   <si>
-    <t>178. $1 &lt;- $0 + 127</t>
-  </si>
-  <si>
     <t>179. if $1 &gt; 0 then pc +=4 + 1</t>
   </si>
   <si>
@@ -191,24 +188,12 @@
     <t>186. $3 &lt;- $3 + 2</t>
   </si>
   <si>
-    <t>187. $0 &lt;- $0 + 126</t>
-  </si>
-  <si>
-    <t>189. $1 &lt;- MEM[$3 + 127]</t>
-  </si>
-  <si>
     <t>190. MEM[$3 + 127] &lt;- $0</t>
   </si>
   <si>
     <t>191. $0 &lt;- $1 + 127</t>
   </si>
   <si>
-    <t>193. $1 &lt;- MEM[$3 + 127]</t>
-  </si>
-  <si>
-    <t>194. $2 &lt;- MEM[$3 + 126]</t>
-  </si>
-  <si>
     <t>195. $0 &lt;- $0 + $1</t>
   </si>
   <si>
@@ -812,6 +797,158 @@
   </si>
   <si>
     <t>37. $1 &lt;- 0 &lt;&lt; 8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>159</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IFID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDEX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXMEM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEMWB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JMP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다음거</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TARGET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>앞에꺼</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>브랜치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> TARGET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>161</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$1 출력</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>씨발!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$3 = 0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$3 = 3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$0 = 0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$0 = 5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$2 = 168</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$1 = 132</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>8e00</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mem[4] = 162</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mem[4] = 5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$3 = 5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$0 = 131</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$2 = 189</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>while ($1 &gt; 0)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mem[4] = $0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$3 += 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>$0 += 126</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mem[3] = 189</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>189. $1 &lt;- MEM[$3 - 1]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>193. $1 &lt;- MEM[$3 - 1]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>178. $1 &lt;- $0 - 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>187. $0 &lt;- $0 - 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>194. $2 &lt;- MEM[$3 - 2]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -819,7 +956,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -844,9 +981,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="8" tint="-0.249977111117893"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -854,7 +1007,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -883,7 +1060,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -893,13 +1070,40 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1184,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:A48"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1207,25 +1411,25 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
@@ -1267,7 +1471,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="L33" s="2">
         <v>0</v>
@@ -1295,15 +1499,16 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="C34" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>253</v>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>248</v>
       </c>
       <c r="G34" s="2">
         <v>0</v>
@@ -1318,12 +1523,12 @@
         <v>3</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="M34" s="5">
+        <v>220</v>
+      </c>
+      <c r="M34" s="3">
         <v>0</v>
       </c>
       <c r="N34" s="2">
@@ -1348,37 +1553,40 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B35" s="2">
+      <c r="A35" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B35" s="10">
         <v>6000</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="G35" s="2">
-        <v>0</v>
-      </c>
-      <c r="H35" s="2">
-        <v>0</v>
-      </c>
-      <c r="I35" s="2">
-        <v>0</v>
-      </c>
-      <c r="J35" s="2">
+      <c r="C35" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="4">
+        <v>0</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0</v>
+      </c>
+      <c r="I35" s="4">
+        <v>0</v>
+      </c>
+      <c r="J35" s="4">
         <v>0</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="N35" s="5">
+        <v>220</v>
+      </c>
+      <c r="N35" s="3">
         <v>0</v>
       </c>
       <c r="O35" s="2">
@@ -1402,32 +1610,35 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G36" s="4">
-        <v>0</v>
-      </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
+      <c r="A36" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="7">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="O36" s="5">
+        <v>220</v>
+      </c>
+      <c r="O36" s="3">
         <v>0</v>
       </c>
       <c r="P36" s="2">
@@ -1450,41 +1661,44 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="B37" s="2">
+      <c r="A37" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B37" s="10">
         <v>6100</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G37" s="2">
-        <v>0</v>
-      </c>
-      <c r="H37" s="2">
-        <v>0</v>
-      </c>
-      <c r="I37" s="2">
-        <v>0</v>
-      </c>
-      <c r="J37" s="2">
+      <c r="C37" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0</v>
+      </c>
+      <c r="J37" s="4">
         <v>0</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="P37" s="5">
+        <v>220</v>
+      </c>
+      <c r="P37" s="3">
         <v>0</v>
       </c>
       <c r="Q37" s="1">
@@ -1504,36 +1718,39 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4">
-        <v>0</v>
-      </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="A38" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7">
+        <v>0</v>
+      </c>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="Q38" s="1">
         <v>0</v>
@@ -1552,42 +1769,45 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="10">
         <v>6200</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G39" s="2">
-        <v>0</v>
-      </c>
-      <c r="H39" s="2">
-        <v>0</v>
-      </c>
-      <c r="I39" s="2">
-        <v>0</v>
-      </c>
-      <c r="J39" s="2">
+      <c r="C39" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0</v>
+      </c>
+      <c r="J39" s="4">
         <v>0</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="Q39" s="1">
         <v>0</v>
@@ -1606,36 +1826,39 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4">
-        <v>0</v>
-      </c>
-      <c r="J40" s="4"/>
+      <c r="A40" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7">
+        <v>0</v>
+      </c>
+      <c r="J40" s="7"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="Q40" s="1">
         <v>0</v>
@@ -1654,42 +1877,45 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="10">
         <v>6300</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G41" s="2">
-        <v>0</v>
-      </c>
-      <c r="H41" s="2">
-        <v>0</v>
-      </c>
-      <c r="I41" s="2">
-        <v>0</v>
-      </c>
-      <c r="J41" s="2">
+      <c r="C41" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="4">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0</v>
+      </c>
+      <c r="J41" s="4">
         <v>0</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="Q41" s="1">
         <v>0</v>
@@ -1708,36 +1934,39 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4">
+      <c r="A42" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7">
         <v>0</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="Q42" s="1">
         <v>0</v>
@@ -1756,42 +1985,45 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="10">
         <v>4401</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G43" s="5">
+      <c r="C43" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="6">
         <v>1</v>
       </c>
-      <c r="H43" s="5">
-        <v>0</v>
-      </c>
-      <c r="I43" s="5">
-        <v>0</v>
-      </c>
-      <c r="J43" s="5">
+      <c r="H43" s="6">
+        <v>0</v>
+      </c>
+      <c r="I43" s="6">
+        <v>0</v>
+      </c>
+      <c r="J43" s="6">
         <v>0</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="Q43" s="1">
         <v>0</v>
@@ -1810,34 +2042,39 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="G44" s="4">
+      <c r="A44" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="7">
         <v>1</v>
       </c>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2">
         <v>4001</v>
       </c>
-      <c r="M44" s="2"/>
+      <c r="M44" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="N44" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="Q44" s="1">
         <v>0</v>
@@ -1856,38 +2093,45 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="10">
         <v>4001</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G45" s="2">
+      <c r="C45" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="4">
         <v>2</v>
       </c>
-      <c r="H45" s="2">
-        <v>0</v>
-      </c>
-      <c r="I45" s="2">
-        <v>0</v>
-      </c>
-      <c r="J45" s="2">
+      <c r="H45" s="4">
+        <v>0</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0</v>
+      </c>
+      <c r="J45" s="4">
         <v>0</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+        <v>158</v>
+      </c>
+      <c r="M45" s="2">
+        <v>4001</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="O45" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="Q45" s="1">
         <v>0</v>
@@ -1906,30 +2150,39 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G46" s="4">
+      <c r="A46" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="7">
         <v>2</v>
       </c>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2">
         <v>5901</v>
       </c>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
+      <c r="M46" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="N46" s="2">
+        <v>4001</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="P46" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="Q46" s="1">
         <v>1</v>
@@ -1948,114 +2201,154 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="10">
         <v>5901</v>
       </c>
-      <c r="G47" s="3">
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="6">
         <v>2</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="6">
         <v>1</v>
       </c>
-      <c r="I47" s="3">
-        <v>0</v>
-      </c>
-      <c r="J47" s="3">
+      <c r="I47" s="6">
+        <v>0</v>
+      </c>
+      <c r="J47" s="6">
         <v>0</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
+      <c r="M47" s="2">
+        <v>5901</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O47" s="2">
+        <v>4001</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2">
+      <c r="A48" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4">
         <v>1</v>
       </c>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
+      <c r="N48" s="2">
+        <v>5901</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="P48" s="2">
+        <v>4001</v>
+      </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="10">
         <v>5502</v>
       </c>
-      <c r="G49" s="2">
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="4">
         <v>2</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49" s="4">
         <v>3</v>
       </c>
-      <c r="I49" s="2">
-        <v>0</v>
-      </c>
-      <c r="J49" s="2">
+      <c r="I49" s="4">
+        <v>0</v>
+      </c>
+      <c r="J49" s="4">
         <v>0</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
+      <c r="O49" s="2">
+        <v>5901</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2">
+      <c r="A50" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="6">
         <v>3</v>
       </c>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
+      <c r="P50" s="2">
+        <v>5901</v>
+      </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="10">
         <v>5503</v>
       </c>
-      <c r="G51" s="2">
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="4">
         <v>2</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51" s="4">
         <v>3</v>
       </c>
-      <c r="I51" s="2">
-        <v>0</v>
-      </c>
-      <c r="J51" s="2">
+      <c r="I51" s="4">
+        <v>0</v>
+      </c>
+      <c r="J51" s="4">
         <v>0</v>
       </c>
       <c r="K51" s="2"/>
@@ -2066,18 +2359,22 @@
       <c r="P51" s="2"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2">
+      <c r="A52" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4">
         <v>3</v>
       </c>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
@@ -2086,12 +2383,15 @@
       <c r="P52" s="2"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>167</v>
-      </c>
+      <c r="B53" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
       <c r="G53" s="2">
         <v>2</v>
       </c>
@@ -2112,12 +2412,15 @@
       <c r="P53" s="2"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A54" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -2132,12 +2435,15 @@
       <c r="P54" s="2"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>168</v>
-      </c>
+      <c r="B55" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
       <c r="G55" s="2">
         <v>2</v>
       </c>
@@ -2158,12 +2464,15 @@
       <c r="P55" s="2"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A56" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -2178,12 +2487,15 @@
       <c r="P56" s="2"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>169</v>
-      </c>
+      <c r="B57" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
       <c r="G57" s="2">
         <v>2</v>
       </c>
@@ -2204,12 +2516,15 @@
       <c r="P57" s="2"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A58" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
@@ -2224,12 +2539,15 @@
       <c r="P58" s="2"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>170</v>
-      </c>
+      <c r="A59" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
       <c r="G59" s="2">
         <v>2</v>
       </c>
@@ -2250,12 +2568,15 @@
       <c r="P59" s="2"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A60" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -2270,12 +2591,15 @@
       <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>171</v>
-      </c>
+      <c r="A61" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
       <c r="G61" s="2">
         <v>2</v>
       </c>
@@ -2296,12 +2620,15 @@
       <c r="P61" s="2"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A62" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -2316,12 +2643,15 @@
       <c r="P62" s="2"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>172</v>
-      </c>
+      <c r="A63" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
       <c r="G63" s="2">
         <v>2</v>
       </c>
@@ -2342,12 +2672,15 @@
       <c r="P63" s="2"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A64" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -2362,12 +2695,15 @@
       <c r="P64" s="2"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>173</v>
-      </c>
+      <c r="A65" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
       <c r="G65" s="2">
         <v>2</v>
       </c>
@@ -2388,12 +2724,15 @@
       <c r="P65" s="2"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A66" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -2408,12 +2747,15 @@
       <c r="P66" s="2"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>174</v>
-      </c>
+      <c r="A67" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -2426,12 +2768,15 @@
       <c r="P67" s="2"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A68" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -2444,12 +2789,15 @@
       <c r="P68" s="2"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>175</v>
-      </c>
+      <c r="A69" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
@@ -2462,12 +2810,15 @@
       <c r="P69" s="2"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A70" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -2480,12 +2831,15 @@
       <c r="P70" s="2"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>176</v>
-      </c>
+      <c r="A71" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -2498,12 +2852,15 @@
       <c r="P71" s="2"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A72" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -2516,12 +2873,15 @@
       <c r="P72" s="2"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>177</v>
-      </c>
+      <c r="A73" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
@@ -2534,12 +2894,15 @@
       <c r="P73" s="2"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A74" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
@@ -2552,12 +2915,15 @@
       <c r="P74" s="2"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>178</v>
-      </c>
+      <c r="A75" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
@@ -2570,12 +2936,15 @@
       <c r="P75" s="2"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A76" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -2588,12 +2957,15 @@
       <c r="P76" s="2"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>179</v>
-      </c>
+      <c r="A77" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -2606,12 +2978,15 @@
       <c r="P77" s="2"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A78" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -2624,12 +2999,15 @@
       <c r="P78" s="2"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>180</v>
-      </c>
+      <c r="A79" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
@@ -2642,12 +3020,15 @@
       <c r="P79" s="2"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A80" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -2660,12 +3041,15 @@
       <c r="P80" s="2"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>181</v>
-      </c>
+      <c r="A81" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
@@ -2678,12 +3062,15 @@
       <c r="P81" s="2"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A82" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
@@ -2696,12 +3083,15 @@
       <c r="P82" s="2"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>182</v>
-      </c>
+      <c r="A83" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -2714,12 +3104,15 @@
       <c r="P83" s="2"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A84" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
@@ -2732,12 +3125,15 @@
       <c r="P84" s="2"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>183</v>
-      </c>
+      <c r="A85" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -2750,12 +3146,15 @@
       <c r="P85" s="2"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A86" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -2768,12 +3167,15 @@
       <c r="P86" s="2"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>184</v>
-      </c>
+      <c r="A87" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -2786,12 +3188,15 @@
       <c r="P87" s="2"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A88" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -2804,12 +3209,15 @@
       <c r="P88" s="2"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>185</v>
-      </c>
+      <c r="A89" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -2822,12 +3230,15 @@
       <c r="P89" s="2"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A90" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
@@ -2840,12 +3251,15 @@
       <c r="P90" s="2"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>186</v>
-      </c>
+      <c r="A91" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
@@ -2858,12 +3272,15 @@
       <c r="P91" s="2"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A92" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
@@ -2876,12 +3293,15 @@
       <c r="P92" s="2"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>187</v>
-      </c>
+      <c r="A93" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
@@ -2894,12 +3314,15 @@
       <c r="P93" s="2"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A94" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
@@ -2912,12 +3335,15 @@
       <c r="P94" s="2"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>188</v>
-      </c>
+      <c r="A95" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -2930,12 +3356,15 @@
       <c r="P95" s="2"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A96" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
@@ -2948,12 +3377,15 @@
       <c r="P96" s="2"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A97" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>189</v>
-      </c>
+      <c r="A97" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
@@ -2966,12 +3398,15 @@
       <c r="P97" s="2"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A98" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A98" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
@@ -2984,12 +3419,15 @@
       <c r="P98" s="2"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>190</v>
-      </c>
+      <c r="A99" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
@@ -3002,12 +3440,15 @@
       <c r="P99" s="2"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A100" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
@@ -3020,12 +3461,15 @@
       <c r="P100" s="2"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>191</v>
-      </c>
+      <c r="A101" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
@@ -3038,408 +3482,612 @@
       <c r="P101" s="2"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A102" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
-      <c r="M102" s="2"/>
-      <c r="N102" s="2"/>
-      <c r="O102" s="2"/>
       <c r="P102" s="2"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>192</v>
-      </c>
+      <c r="A103" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
-      <c r="L103" s="2"/>
-      <c r="M103" s="2"/>
-      <c r="N103" s="2"/>
-      <c r="O103" s="2"/>
       <c r="P103" s="2"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A104" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>166</v>
+      <c r="A104" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
-      <c r="L104" s="2"/>
-      <c r="M104" s="2"/>
-      <c r="N104" s="2"/>
-      <c r="O104" s="2"/>
       <c r="P104" s="2"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>193</v>
-      </c>
+      <c r="A105" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
       <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
+      <c r="H105" s="2" t="s">
+        <v>255</v>
+      </c>
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
-      <c r="L105" s="2"/>
-      <c r="M105" s="2"/>
-      <c r="N105" s="2"/>
-      <c r="O105" s="2"/>
       <c r="P105" s="2"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>166</v>
-      </c>
+      <c r="A106" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
+      <c r="H106" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
-      <c r="L106" s="2"/>
-      <c r="M106" s="2"/>
-      <c r="N106" s="2"/>
-      <c r="O106" s="2"/>
       <c r="P106" s="2"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B107" s="10">
         <v>7801</v>
       </c>
+      <c r="C107" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F107" s="2"/>
       <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
+      <c r="H107" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="K107" s="2"/>
-      <c r="L107" s="2"/>
-      <c r="M107" s="2"/>
-      <c r="N107" s="2"/>
-      <c r="O107" s="2"/>
       <c r="P107" s="2"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>163</v>
+      <c r="A108" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-      <c r="K108" s="2"/>
-      <c r="L108" s="2"/>
-      <c r="M108" s="2"/>
-      <c r="N108" s="2"/>
-      <c r="O108" s="2"/>
+      <c r="I108" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="P108" s="2"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A109" s="2" t="s">
+      <c r="A109" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B109" s="10">
         <v>7902</v>
+      </c>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-      <c r="K109" s="2"/>
-      <c r="L109" s="2"/>
-      <c r="M109" s="2"/>
-      <c r="N109" s="2"/>
-      <c r="O109" s="2"/>
+      <c r="J109" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="K109" s="2" t="s">
+        <v>256</v>
+      </c>
       <c r="P109" s="2"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>164</v>
+      <c r="A110" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
-      <c r="L110" s="2"/>
-      <c r="M110" s="2"/>
-      <c r="N110" s="2"/>
-      <c r="O110" s="2"/>
+      <c r="K110" s="2" t="s">
+        <v>258</v>
+      </c>
       <c r="P110" s="2"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B111" s="8">
         <v>8901</v>
       </c>
-      <c r="G111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
-      <c r="L111" s="2"/>
-      <c r="M111" s="2"/>
-      <c r="N111" s="2"/>
       <c r="O111" s="2"/>
       <c r="P111" s="2"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B112" s="8">
         <v>8802</v>
       </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
-      <c r="L112" s="2"/>
-      <c r="M112" s="2"/>
-      <c r="N112" s="2"/>
       <c r="O112" s="2"/>
       <c r="P112" s="2"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113" s="8">
         <v>7801</v>
       </c>
+      <c r="C113" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
-      <c r="L113" s="2"/>
-      <c r="M113" s="2"/>
-      <c r="N113" s="2"/>
       <c r="O113" s="2"/>
       <c r="P113" s="2"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A114" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>163</v>
+      <c r="A114" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
-      <c r="L114" s="2"/>
-      <c r="M114" s="2"/>
-      <c r="N114" s="2"/>
       <c r="O114" s="2"/>
       <c r="P114" s="2"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B115" s="8">
         <v>7902</v>
       </c>
+      <c r="C115" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
       <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
+      <c r="H115" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
-      <c r="L115" s="2"/>
+      <c r="L115" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
       <c r="O115" s="2"/>
       <c r="P115" s="2"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>164</v>
-      </c>
+      <c r="A116" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
       <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
+      <c r="H116" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
-      <c r="L116" s="2"/>
-      <c r="M116" s="2"/>
+      <c r="L116" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="M116" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="N116" s="2"/>
       <c r="O116" s="2"/>
       <c r="P116" s="2"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B117" s="13">
         <v>9076</v>
       </c>
+      <c r="C117" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F117" s="2"/>
       <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
-      <c r="I117" s="2"/>
-      <c r="J117" s="2"/>
+      <c r="H117" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="K117" s="2"/>
-      <c r="L117" s="2"/>
-      <c r="M117" s="2"/>
-      <c r="N117" s="2"/>
+      <c r="L117" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N117" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="O117" s="2"/>
       <c r="P117" s="2"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>163</v>
+      <c r="A118" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B118" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>260</v>
       </c>
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
-      <c r="J118" s="2"/>
-      <c r="K118" s="2"/>
-      <c r="L118" s="2"/>
-      <c r="M118" s="2"/>
-      <c r="N118" s="2"/>
-      <c r="O118" s="2"/>
+      <c r="J118" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="K118" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N118" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="O118" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="P118" s="2"/>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B119" s="13">
         <v>9079</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
       <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
-      <c r="L119" s="2"/>
-      <c r="M119" s="2"/>
-      <c r="N119" s="2"/>
-      <c r="O119" s="2"/>
+      <c r="K119" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="L119" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="N119" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="O119" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="P119" s="2"/>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>194</v>
+      <c r="A120" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B120" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
-      <c r="L120" s="2"/>
-      <c r="M120" s="2"/>
-      <c r="N120" s="2"/>
-      <c r="O120" s="2"/>
+      <c r="L120" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="M120" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="N120" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="O120" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="P120" s="2"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>164</v>
+      <c r="A121" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B121" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
-      <c r="L121" s="2"/>
-      <c r="M121" s="2"/>
-      <c r="N121" s="2"/>
-      <c r="O121" s="2"/>
+      <c r="M121" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="N121" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="O121" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="P121" s="2"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A122" s="2" t="s">
+      <c r="A122" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>195</v>
+      <c r="B122" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
-      <c r="L122" s="2"/>
-      <c r="M122" s="2"/>
-      <c r="N122" s="2"/>
-      <c r="O122" s="2"/>
+      <c r="N122" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="O122" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="P122" s="2"/>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>196</v>
+      <c r="B123" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2" t="s">
+        <v>258</v>
       </c>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
-      <c r="L123" s="2"/>
-      <c r="M123" s="2"/>
-      <c r="N123" s="2"/>
-      <c r="O123" s="2"/>
+      <c r="O123" s="2" t="s">
+        <v>258</v>
+      </c>
       <c r="P123" s="2"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A124" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>194</v>
-      </c>
+      <c r="A124" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B124" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C124" s="14"/>
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
@@ -3452,11 +4100,23 @@
       <c r="P124" s="2"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A125" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>163</v>
+      <c r="A125" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B125" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C125" s="14">
+        <v>65535</v>
+      </c>
+      <c r="D125" s="1">
+        <v>1</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0</v>
+      </c>
+      <c r="F125" s="1">
+        <v>0</v>
       </c>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
@@ -3470,12 +4130,13 @@
       <c r="P125" s="2"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A126" s="2" t="s">
+      <c r="A126" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B126" s="2">
+      <c r="B126" s="13">
         <v>601</v>
       </c>
+      <c r="C126" s="14"/>
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
@@ -3488,12 +4149,13 @@
       <c r="P126" s="2"/>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A127" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>194</v>
-      </c>
+      <c r="A127" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C127" s="14"/>
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
@@ -3506,12 +4168,13 @@
       <c r="P127" s="2"/>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A128" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>164</v>
-      </c>
+      <c r="A128" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C128" s="14"/>
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
@@ -3524,12 +4187,13 @@
       <c r="P128" s="2"/>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B129" s="2">
+      <c r="B129" s="13">
         <v>1601</v>
       </c>
+      <c r="C129" s="14"/>
       <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
@@ -3542,12 +4206,13 @@
       <c r="P129" s="2"/>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B130" s="2">
+      <c r="B130" s="13">
         <v>9084</v>
       </c>
+      <c r="C130" s="14"/>
       <c r="G130" s="2"/>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
@@ -3560,12 +4225,13 @@
       <c r="P130" s="2"/>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A131" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>194</v>
-      </c>
+      <c r="A131" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B131" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C131" s="14"/>
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
@@ -3578,12 +4244,13 @@
       <c r="P131" s="2"/>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>163</v>
-      </c>
+      <c r="A132" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B132" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C132" s="14"/>
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
@@ -3596,12 +4263,13 @@
       <c r="P132" s="2"/>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A133" s="2" t="s">
+      <c r="A133" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>197</v>
-      </c>
+      <c r="B133" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C133" s="14"/>
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
@@ -3614,12 +4282,13 @@
       <c r="P133" s="2"/>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A134" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>194</v>
-      </c>
+      <c r="A134" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B134" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C134" s="14"/>
       <c r="G134" s="2"/>
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
@@ -3632,12 +4301,13 @@
       <c r="P134" s="2"/>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>164</v>
-      </c>
+      <c r="A135" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B135" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C135" s="14"/>
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
@@ -3650,11 +4320,14 @@
       <c r="P135" s="2"/>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A136" s="2" t="s">
+      <c r="A136" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B136" s="2">
+      <c r="B136" s="13">
         <v>2001</v>
+      </c>
+      <c r="C136" s="14">
+        <v>-1</v>
       </c>
       <c r="G136" s="2"/>
       <c r="H136" s="2"/>
@@ -3672,7 +4345,7 @@
         <v>7</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
@@ -3687,10 +4360,10 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G138" s="2"/>
       <c r="H138" s="2"/>
@@ -3705,10 +4378,10 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
@@ -3741,10 +4414,10 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
@@ -3759,10 +4432,10 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G142" s="2"/>
       <c r="H142" s="2"/>
@@ -3813,10 +4486,10 @@
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
@@ -3831,10 +4504,10 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
@@ -3867,10 +4540,10 @@
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
@@ -3885,10 +4558,10 @@
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
@@ -3939,10 +4612,10 @@
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
@@ -3957,10 +4630,10 @@
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
@@ -3996,7 +4669,7 @@
         <v>11</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
@@ -4011,10 +4684,10 @@
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
@@ -4029,10 +4702,10 @@
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
@@ -4050,10 +4723,12 @@
         <v>12</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C158" s="2"/>
-      <c r="D158" s="2"/>
+      <c r="D158" s="2" t="s">
+        <v>250</v>
+      </c>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
       <c r="G158" s="2"/>
@@ -4065,10 +4740,10 @@
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
@@ -4086,10 +4761,12 @@
         <v>13</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
+      <c r="D160" s="2" t="s">
+        <v>263</v>
+      </c>
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
       <c r="G160" s="2"/>
@@ -4101,10 +4778,10 @@
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
@@ -4119,13 +4796,15 @@
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C162" s="2"/>
-      <c r="D162" s="2"/>
+      <c r="D162" s="2" t="s">
+        <v>264</v>
+      </c>
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
@@ -4143,7 +4822,9 @@
         <v>6300</v>
       </c>
       <c r="C163" s="2"/>
-      <c r="D163" s="2"/>
+      <c r="D163" s="2" t="s">
+        <v>266</v>
+      </c>
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
@@ -4158,10 +4839,12 @@
         <v>47</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C164" s="2"/>
-      <c r="D164" s="2"/>
+      <c r="D164" s="2" t="s">
+        <v>267</v>
+      </c>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
@@ -4179,7 +4862,9 @@
         <v>6000</v>
       </c>
       <c r="C165" s="2"/>
-      <c r="D165" s="2"/>
+      <c r="D165" s="2" t="s">
+        <v>268</v>
+      </c>
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
@@ -4197,7 +4882,9 @@
         <v>4005</v>
       </c>
       <c r="C166" s="2"/>
-      <c r="D166" s="2"/>
+      <c r="D166" s="2" t="s">
+        <v>269</v>
+      </c>
       <c r="E166" s="2"/>
       <c r="F166" s="2"/>
       <c r="G166" s="2"/>
@@ -4212,10 +4899,12 @@
         <v>16</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C167" s="2"/>
-      <c r="D167" s="2"/>
+      <c r="D167" s="2" t="s">
+        <v>270</v>
+      </c>
       <c r="E167" s="2"/>
       <c r="F167" s="2"/>
       <c r="G167" s="2"/>
@@ -4227,10 +4916,10 @@
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
@@ -4248,7 +4937,7 @@
         <v>17</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
@@ -4281,10 +4970,10 @@
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
@@ -4299,10 +4988,10 @@
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
@@ -4317,10 +5006,10 @@
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
@@ -4338,13 +5027,15 @@
         <v>49</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
-      <c r="G174" s="2"/>
+      <c r="G174" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="H174" s="2"/>
       <c r="I174" s="2"/>
       <c r="J174" s="2"/>
@@ -4353,10 +5044,10 @@
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
@@ -4371,13 +5062,15 @@
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C176" s="2"/>
-      <c r="D176" s="2"/>
+      <c r="D176" s="2" t="s">
+        <v>265</v>
+      </c>
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
@@ -4392,13 +5085,15 @@
         <v>18</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
-      <c r="G177" s="2"/>
+      <c r="G177" s="2" t="s">
+        <v>271</v>
+      </c>
       <c r="H177" s="2"/>
       <c r="I177" s="2"/>
       <c r="J177" s="2"/>
@@ -4407,16 +5102,20 @@
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
-        <v>50</v>
+        <v>285</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C178" s="2"/>
-      <c r="D178" s="2"/>
+      <c r="D178" s="2" t="s">
+        <v>271</v>
+      </c>
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
-      <c r="G178" s="2"/>
+      <c r="G178" s="2" t="s">
+        <v>278</v>
+      </c>
       <c r="H178" s="2"/>
       <c r="I178" s="2"/>
       <c r="J178" s="2"/>
@@ -4425,7 +5124,7 @@
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B179" s="2">
         <v>2404</v>
@@ -4434,7 +5133,9 @@
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
-      <c r="G179" s="2"/>
+      <c r="G179" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="H179" s="2"/>
       <c r="I179" s="2"/>
       <c r="J179" s="2"/>
@@ -4452,7 +5153,9 @@
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
       <c r="F180" s="2"/>
-      <c r="G180" s="2"/>
+      <c r="G180" s="2" t="s">
+        <v>279</v>
+      </c>
       <c r="H180" s="2"/>
       <c r="I180" s="2"/>
       <c r="J180" s="2"/>
@@ -4470,7 +5173,9 @@
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
       <c r="F181" s="2"/>
-      <c r="G181" s="2"/>
+      <c r="G181" s="2" t="s">
+        <v>280</v>
+      </c>
       <c r="H181" s="2"/>
       <c r="I181" s="2"/>
       <c r="J181" s="2"/>
@@ -4479,16 +5184,18 @@
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
-      <c r="G182" s="2"/>
+      <c r="G182" s="2" t="s">
+        <v>281</v>
+      </c>
       <c r="H182" s="2"/>
       <c r="I182" s="2"/>
       <c r="J182" s="2"/>
@@ -4497,10 +5204,10 @@
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
@@ -4515,13 +5222,15 @@
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B184" s="2">
-        <v>8</v>
+        <v>51</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="C184" s="2"/>
-      <c r="D184" s="2"/>
+      <c r="D184" s="2" t="s">
+        <v>273</v>
+      </c>
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
@@ -4533,13 +5242,15 @@
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C185" s="2"/>
-      <c r="D185" s="2"/>
+      <c r="D185" s="2" t="s">
+        <v>274</v>
+      </c>
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
@@ -4551,13 +5262,15 @@
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C186" s="2"/>
-      <c r="D186" s="2"/>
+      <c r="D186" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
@@ -4569,13 +5282,15 @@
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
-        <v>55</v>
+        <v>286</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C187" s="2"/>
-      <c r="D187" s="2"/>
+      <c r="D187" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
       <c r="G187" s="2"/>
@@ -4590,10 +5305,12 @@
         <v>21</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C188" s="2"/>
-      <c r="D188" s="2"/>
+      <c r="D188" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
@@ -4605,10 +5322,10 @@
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
-        <v>56</v>
+        <v>283</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
@@ -4623,10 +5340,10 @@
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
@@ -4641,10 +5358,10 @@
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
@@ -4662,7 +5379,7 @@
         <v>22</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
@@ -4677,10 +5394,10 @@
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
-        <v>59</v>
+        <v>284</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
@@ -4695,10 +5412,10 @@
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
-        <v>60</v>
+        <v>287</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
@@ -4713,10 +5430,10 @@
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
@@ -4731,10 +5448,10 @@
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
@@ -4749,10 +5466,10 @@
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
@@ -4767,10 +5484,10 @@
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>

</xml_diff>